<commit_message>
make correction in switch chat service
</commit_message>
<xml_diff>
--- a/src/main/resources/files/CampaignPersonalised.xlsx
+++ b/src/main/resources/files/CampaignPersonalised.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91757\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91757\Desktop\ChatAI\ChatAI\src\main\resources\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9629C39-66D0-420B-BD64-12ED44F71F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27463E27-D088-40AE-A139-84D90DB9A9EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="56">
   <si>
     <t>Salaried</t>
   </si>
@@ -36,161 +36,170 @@
     <t>whatsapp</t>
   </si>
   <si>
-    <t>Maximize Savings Today</t>
-  </si>
-  <si>
-    <t>Boost FD returns easily!</t>
-  </si>
-  <si>
-    <t>The message targets a salaried individual who values security and stability in their financial transactions, as indicated by their preference for savings and Fixed Deposit (FD) accounts over riskier investment options like credit cards or internet banking. The use of 'Maximize Savings Today' appeals to their desire for financial growth and security. 'Boost FD returns easily!' emphasizes the convenience and benefits of increasing their returns on existing FD accounts, encouraging them to take a proactive step in managing their finances without the need for additional banking services.</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
-    <t>null</t>
-  </si>
-  <si>
     <t>notification</t>
   </si>
   <si>
     <t>Maximize Your Savings</t>
   </si>
   <si>
-    <t>Earn more with FD offers!</t>
-  </si>
-  <si>
-    <t>Given that the user is a salaried individual with a savings and fixed deposit (FD) account at Bank of Baroda, they likely prioritize financial stability and growth. The archetype 'ruler' suggests they appreciate control and security. The user rarely uses their ATM card and does not engage with internet banking or credit services, indicating a preference for traditional banking methods. The message encourages the user to capitalize on FD offers to enhance their savings, aligning with their financial goals and preferences for secure, controlled investment options.</t>
-  </si>
-  <si>
     <t>Marketing</t>
   </si>
   <si>
-    <t>Optimize Your Savings</t>
-  </si>
-  <si>
-    <t>Maximize FD returns now!</t>
-  </si>
-  <si>
-    <t>Given the archetype of the user as a 'Ruler,' the messaging should focus on control and optimization. This user has a saving and FD account, indicating a preference for secure, high-yield investments. The minimal use of the ATM card and lack of internet banking or credit usage suggests a conservative approach to finances. Therefore, the message encourages the user to maximize their returns, appealing to their desire for control and efficiency in managing their savings and investments. This aligns with their financial behavior and encourages further engagement with the bank's offerings.</t>
-  </si>
-  <si>
-    <t>Maximize Your Earnings</t>
-  </si>
-  <si>
-    <t>Boost FD Returns Today</t>
-  </si>
-  <si>
-    <t>This notification is targeted at a salaried individual who has a savings and fixed deposit (FD) account with Bank of Baroda, and uses an ATM card sparingly. The archetype 'Ruler' values control, stability, and growth, making the message 'Maximize Your Earnings' appealing. The subtext 'Boost FD Returns Today' prompts the user to take action and optimize their fixed deposit returns, aligning with their financial goals and preference for secure, high-yield investments. This approach leverages their existing relationship with the bank and encourages deeper engagement with FD products.</t>
-  </si>
-  <si>
-    <t>Unlock exclusive benefits today</t>
-  </si>
-  <si>
-    <t>The 'Ruler' archetype values control and stability, making it essential to highlight the benefits of maximizing savings and taking control of their financial growth. By focusing on exclusive benefits, it appeals to their desire for exclusivity and superior service. The message encourages the use of existing savings and FD accounts, while subtly nudging towards the utilization of additional banking services for greater financial empowerment. This approach aligns with their preference for reliability and control over their financial decisions.</t>
-  </si>
-  <si>
     <t>Retired</t>
   </si>
   <si>
-    <t>Secure Your Savings</t>
-  </si>
-  <si>
-    <t>Ensure your FD's safety.</t>
-  </si>
-  <si>
-    <t>The archetype 'Ruler' typically values stability, control, and security. This retired individual has both a savings and FD account, signifying a preference for secure and reliable financial products. Highlighting the security of their Fixed Deposits (FDs) reassures them of their financial stability. Given that they rarely use their ATM card and have no internet banking or credit usage, the message emphasizes safety, a primary concern for someone who values control and security in their financial matters.</t>
-  </si>
-  <si>
-    <t>Ensure your funds are safe</t>
-  </si>
-  <si>
-    <t>The archetype of a ruler suggests that the retired person values control and security over their finances. By emphasizing the safety and security of their savings, the message aligns with their desire for stability. The subtext reassures them that Bank of Baroda is committed to keeping their funds protected, which is crucial for someone who may not frequently use their ATM card or engage in internet banking. This message builds trust and reinforces the bank’s role in safeguarding their hard-earned money.</t>
-  </si>
-  <si>
-    <t>Secure Your Legacy</t>
-  </si>
-  <si>
-    <t>Enhanced savings &amp; FD benefits</t>
-  </si>
-  <si>
-    <t>The 'Ruler' archetype values security, control, and stability. The heading 'Secure Your Legacy' resonates with their desire to protect and build their financial legacy. The subtext 'Enhanced savings &amp; FD benefits' highlights improvements in areas that are relevant to their existing relationship with the bank, such as saving and fixed deposit accounts. This message encourages them to review and potentially take advantage of new benefits, reinforcing the trust and reliability they seek from Bank of Baroda.</t>
-  </si>
-  <si>
-    <t>Exclusive FD rates for you!</t>
-  </si>
-  <si>
-    <t>The retired person archetype, 'ruler,' values control, stability, and the assurance of their financial decisions. Given their preference for savings and FD accounts, they are likely to appreciate opportunities to maximize their savings. Highlighting exclusive FD rates directly appeals to their desire for financial growth and security without needing to rely on digital banking or credit usage. This message reassures them that they are valued and offers a tangible benefit aligned with their interests.</t>
-  </si>
-  <si>
-    <t>Exclusive FD rates for you</t>
-  </si>
-  <si>
-    <t>Given the user's archetype as a ruler and their preference for traditional banking methods such as savings and fixed deposits (FDs), the notification aims to highlight the benefits of maximizing their savings with Bank of Baroda. The heading 'Maximize Your Savings' appeals to their desire for control and stability, while the subtext 'Exclusive FD rates for you' suggests a personalized offer, making them feel valued and in control of their financial future. This approach aligns with their existing banking habits and encourages them to engage more with their FD account.</t>
-  </si>
-  <si>
-    <t>Boost returns with our FD plans</t>
-  </si>
-  <si>
-    <t>The message addresses a retired person with savings and FD accounts, aiming to highlight an opportunity for better returns. The heading 'Maximize Your Savings' appeals to the Ruler archetype's need for control and stability, suggesting an actionable step to secure their financial future. The subtext 'Boost returns with our FD plans' emphasizes the specific product (FD) that aligns with their existing preferences and financial habits, encouraging further engagement without the need for internet banking or credit usage.</t>
-  </si>
-  <si>
     <t>Freshers</t>
   </si>
   <si>
-    <t>Exclusive offers for FD holders</t>
-  </si>
-  <si>
-    <t>The 'Ruler' archetype appreciates control and stability, making them ideal candidates for maximizing savings through secure investments like Fixed Deposits (FDs). Given that this customer has both a savings and FD account, the message emphasizes exclusive offers tailored to enhance their savings. This approach not only aligns with their preference for control and financial security but also encourages them to engage more actively with their FD account, thus increasing their overall satisfaction with Bank of Baroda.</t>
-  </si>
-  <si>
-    <t>Secure Your Future</t>
-  </si>
-  <si>
-    <t>Maximize FD returns safely.</t>
-  </si>
-  <si>
-    <t>The 'Ruler' archetype values control, stability, and security. This notification aims to reinforce the benefits of their existing Fixed Deposit (FD) account, appealing to their desire for a well-structured and secure financial future. By highlighting the safety and returns of FD, the message aligns with their preference for low-risk investments and reinforces their decision to bank with Bank of Baroda. The straightforward and authoritative language resonates with their need for control and reliability in their banking choices.</t>
-  </si>
-  <si>
-    <t>Explore FD with higher returns</t>
-  </si>
-  <si>
-    <t>Given that the user is a 'Ruler' archetype, they value control, stability, and maximizing their financial growth. The user also has both a savings and FD account, indicating a preference for secure and stable investments. The heading 'Maximize Your Savings' appeals to their desire for control and growth, while the subtext 'Explore FD with higher returns' provides a clear, concise call to action that aligns with their financial goals. The message is crafted to encourage the user to leverage their existing FD account for potentially higher returns, aligning with their preference for stability and growth.</t>
-  </si>
-  <si>
-    <t>Empower Your Savings</t>
-  </si>
-  <si>
-    <t>Boost control with FD</t>
-  </si>
-  <si>
-    <t>The heading 'Empower Your Savings' resonates with the Ruler archetype, who values control and authority. The subtext 'Boost control with FD' encourages the user to leverage their Fixed Deposit (FD) account, emphasizing the control and growth potential it offers. By focusing on their existing savings and FD accounts, the message appeals to their desire for stability and empowerment without introducing unfamiliar banking products like internet banking or credit cards. This approach is aligned with their current banking habits and preferences, ensuring the message is relevant and motivating.</t>
-  </si>
-  <si>
-    <t>Maximize Your Wealth</t>
-  </si>
-  <si>
-    <t>Unlock exclusive benefits today.</t>
-  </si>
-  <si>
-    <t>The heading 'Maximize Your Wealth' directly appeals to the 'Ruler' archetype, who values control, organization, and the efficient management of resources. The subtext 'Unlock exclusive benefits today' entices the user to engage more with Bank of Baroda's services, leveraging their existing savings and FD accounts. This approach is designed to encourage the user to utilize their ATM card more frequently and explore additional financial products, aligning with their desire for maximizing wealth and optimizing financial management.</t>
-  </si>
-  <si>
-    <t>Maximize Your Benefits</t>
-  </si>
-  <si>
-    <t>Leverage your savings and FD now!</t>
-  </si>
-  <si>
-    <t>The 'Ruler' archetype values control, stability, and efficiency. By highlighting the benefits of their existing savings and FD accounts, the message appeals to their desire for maximizing returns. The call to action encourages them to take advantage of the benefits they already have, fostering a sense of empowerment. This strategic approach aims to increase engagement with the bank's offerings while catering to the archetype's preference for structured and reliable financial growth.</t>
+    <t>💼 Secure Your Future with BoB!</t>
+  </si>
+  <si>
+    <t>Enjoy exclusive benefits with your BoB Savings &amp; FD accounts. Activate your ATM for added convenience!</t>
+  </si>
+  <si>
+    <t>The messaging targets a salaried person with a 'Ruler' archetype, emphasizing control and security. It highlights the exclusive benefits of their existing accounts, encouraging the use of their ATM card for convenience. This approach aligns with their desire for stability and control over their financial future, while subtly promoting more engagement with bank services.</t>
+  </si>
+  <si>
+    <t>Maximize Your Savings with Bank of Baroda</t>
+  </si>
+  <si>
+    <t>Unlock exclusive benefits by activating your ATM card and explore our convenient digital banking solutions today!</t>
+  </si>
+  <si>
+    <t>The 'Ruler' archetype values control, leadership, and security. This email appeals to these traits by emphasizing the potential to 'maximize savings' and 'unlock exclusive benefits,' which aligns with their desire for control over their finances. By mentioning the rarely used ATM card and suggesting an exploration of digital banking solutions, the copy aims to introduce convenient options that enhance their banking experience, making it more efficient and secure. Highlighting 'exclusive benefits' and 'digital solutions' addresses their preference for premium services and cutting-edge financial management tools.</t>
+  </si>
+  <si>
+    <t>Exclusive FD rates for you.</t>
+  </si>
+  <si>
+    <t>Targeted at salaried individuals with a savings and FD account at Bank of Baroda, this notification encourages further engagement with the bank's FD products. The user, who rarely uses their ATM card and has no internet banking or credit usage, is likely to be interested in secure and stable investment options. Highlighting exclusive FD rates caters to their financial prudence and desire for solid returns, reinforcing their trust and loyalty towards the bank.</t>
+  </si>
+  <si>
+    <t>👑 Maximize Your Savings with BoB! 💰</t>
+  </si>
+  <si>
+    <t>Hi [Name], unlock higher returns with our exclusive FD rates! Visit your branch today.</t>
+  </si>
+  <si>
+    <t>The 'Ruler' archetype values control, stability, and leadership. This message appeals to their desire for maximizing financial growth and making informed decisions. By emphasizing the exclusive FD rates, it encourages a visit to the branch, fitting their preference for personal interactions over digital channels. The use of emojis adds a personal touch and makes the message more engaging, aligning with their status-conscious nature.</t>
+  </si>
+  <si>
+    <t>Empower Your Finances with Exclusive Digital Services</t>
+  </si>
+  <si>
+    <t>Maximize your savings and investments with Bank of Baroda’s seamless online banking. Activate now and enjoy control at your fingertips.</t>
+  </si>
+  <si>
+    <t>The email targets a salaried individual with a ruler archetype, who values control and empowerment. The heading emphasizes empowerment, aligning with the ruler's desire for control and authority. The subtext highlights the benefits of online banking, such as maximizing savings and investments, which appeals to their goal-oriented nature. Encouraging activation of digital services aims to increase engagement with the bank’s offerings and improve customer experience, by providing the convenience and control they value.</t>
+  </si>
+  <si>
+    <t>Unlock higher FD rates</t>
+  </si>
+  <si>
+    <t>The notification aims to resonate with the 'Ruler' archetype's desire for control and stability. Highlighting the benefit of higher FD rates appeals to their practical and security-oriented mindset. This user, who has both a savings and FD account but rarely uses their ATM card, is likely focused on long-term financial growth rather than day-to-day transactions. By emphasizing the opportunity to maximize their savings, we address their preference for structured and reliable financial products, encouraging them to engage more with the bank's offerings.</t>
+  </si>
+  <si>
+    <t>Optimize Your Savings with Us! 💼</t>
+  </si>
+  <si>
+    <t>Dear Valued Customer, explore higher returns with our Senior Citizen FD rates! 📈</t>
+  </si>
+  <si>
+    <t>The target audience is a retired person, categorized as a 'ruler' archetype who likely values stability and control over their finances. This individual has existing savings and FD accounts with the Bank of Baroda, and rarely uses their ATM card. By highlighting the attractive FD rates specifically for senior citizens, the message aims to resonate with their desire for optimal financial management and higher returns. The use of emojis adds a friendly touch while keeping the message concise and appealing.</t>
+  </si>
+  <si>
+    <t>Enhance Your Savings with Bank of Baroda!</t>
+  </si>
+  <si>
+    <t>Dear Valued Customer, discover exclusive benefits for your savings &amp; FD accounts. Visit your nearest branch today!</t>
+  </si>
+  <si>
+    <t>The email is designed to appeal to the 'Ruler' archetype, emphasizing control and benefits. The heading highlights the opportunity to enhance savings, which appeals to their desire for security and growth. The subtext encourages a visit to the branch, aligning with the user's preference for in-person banking rather than online services. This personalized approach reassures the retired customer of the bank's commitment to providing tailored financial solutions.</t>
+  </si>
+  <si>
+    <t>Exclusive FD rates for loyal customers</t>
+  </si>
+  <si>
+    <t>Given the archetype of a 'ruler,' the retired customer values stability and control over their finances. Emphasizing the opportunity to 'maximize savings' appeals to the desire for financial prudence and security. Highlighting 'exclusive FD rates for loyal customers' leverages the personal connection the customer has with the bank, acknowledging their long-term relationship and loyalty. This messaging is concise and directly relevant to the customer's existing saving and FD accounts, encouraging further investment without reference to services they rarely use, such as ATM cards or internet banking.</t>
+  </si>
+  <si>
+    <t>👑 Secure Your Legacy</t>
+  </si>
+  <si>
+    <t>Enjoy premium FD rates &amp; personalized services. Visit us!</t>
+  </si>
+  <si>
+    <t>The message targets a retired 'ruler' archetype, emphasizing control and security. Highlighting premium FD rates appeals to their interest in financial stability, while personalized services cater to their desire for tailored, high-quality service. Encouraging a visit aligns with their preference for face-to-face interactions over digital services.</t>
+  </si>
+  <si>
+    <t>Maximize Your Savings with Exclusive Offers!</t>
+  </si>
+  <si>
+    <t>Dear Esteemed Customer, enjoy higher returns on your FD and special benefits on your savings account. Act now to secure your financial future.</t>
+  </si>
+  <si>
+    <t>The email is designed to appeal to the 'Ruler' archetype, emphasizing control and security. Using terms like 'maximize,' 'higher returns,' and 'secure your financial future,' aligns with their need for stability and prudence. Highlighting exclusive offers and benefits on existing FD and savings accounts ensures the message resonates with their desire for exclusivity and wise management of their resources. The call to action encourages immediate engagement, tapping into their proactive nature.</t>
+  </si>
+  <si>
+    <t>Exclusive benefits for your FD account</t>
+  </si>
+  <si>
+    <t>The notification aims to appeal to a retired person who values control and stability (ruler archetype). By highlighting exclusive benefits for his Fixed Deposit (FD) account, the message resonates with his desire for financial security and maximization of savings. Since he rarely uses his ATM card, the focus is kept on savings and FD, which are more relevant to his financial behavior and preferences. This approach encourages him to engage more with his existing accounts, ensuring he feels valued and informed about opportunities to grow his wealth.</t>
+  </si>
+  <si>
+    <t>Unlock Your Financial Potential 💼✨</t>
+  </si>
+  <si>
+    <t>Maximize your savings and FD returns with exclusive offers. Start using your ATM card more often!</t>
+  </si>
+  <si>
+    <t>Considering the archetype of the ruler, who values control and stability, the message emphasizes maximizing financial returns and leveraging existing banking facilities. The freshers' status indicates the need for financial growth and security. By highlighting savings and FD account benefits and encouraging the use of the ATM card, the message aligns with their preference for practical and controlled financial management. The use of emojis adds a friendly and engaging touch.</t>
+  </si>
+  <si>
+    <t>Enhance your savings experience with our exclusive offers. Activate internet banking today and enjoy seamless financial management.</t>
+  </si>
+  <si>
+    <t>The email is crafted for a 'Ruler' archetype, which values control and efficiency. By highlighting the benefits of internet banking, the email appeals to the user's desire for streamlined financial management. Additionally, the mention of 'exclusive offers' can pique interest and encourage action. Given that the user rarely uses their ATM card, the email focuses on the convenience and enhanced control provided by internet banking, which aligns with their profile and preferences.</t>
+  </si>
+  <si>
+    <t>Unlock FD benefits now</t>
+  </si>
+  <si>
+    <t>This notification is designed to appeal to a 'Ruler' archetype who values control and authority over their finances. By emphasizing the benefits of their Fixed Deposit (FD) account, we encourage them to maximize their returns. This also subtly nudges them to engage more actively with their Bank of Baroda accounts. The compact, action-oriented copy aligns with their decisive nature, while the mention of unlocking benefits taps into their desire for financial growth and optimization.</t>
+  </si>
+  <si>
+    <t>💼 Manage Your Wealth Effortlessly!</t>
+  </si>
+  <si>
+    <t>Hello, Neeraj! Simplify your banking with Bank of Baroda's mobile app. Track savings, FD, and more! 📱</t>
+  </si>
+  <si>
+    <t>Neeraj embodies the 'Ruler' archetype, valuing control and stability. Despite having savings, FD, and an ATM card, he lacks efficient management tools like internet banking. This message highlights the convenience of the Bank of Baroda mobile app, encouraging him to take charge of his finances effortlessly. The use of emojis adds a friendly touch, making the offer appealing and relatable.</t>
+  </si>
+  <si>
+    <t>Dear Valued Customer, Boost your savings and enjoy exclusive benefits with your Bank of Baroda accounts. Activate your ATM card today and explore our digital banking services for a seamless experience.</t>
+  </si>
+  <si>
+    <t>The email targets a fresher with a 'Ruler' archetype, focusing on control and efficiency. By highlighting the potential to 'maximize savings' and 'exclusive benefits,' the message appeals to their desire for control over their financial growth. Encouraging ATM card activation and digital banking adoption addresses their current underutilization, providing them with tools to better manage and monitor their finances.</t>
+  </si>
+  <si>
+    <t>Enhance Your Control</t>
+  </si>
+  <si>
+    <t>Activate Internet Banking Today!</t>
+  </si>
+  <si>
+    <t>Given the user's archetype as a 'Ruler,' they value control and authority. The notification encourages them to enhance their control over their finances by activating internet banking. This service can provide them with comprehensive oversight and management of their savings and FD accounts, which aligns with their desire for control. Additionally, emphasizing the activation aspect appeals to their proactive nature, making them feel empowered to take charge of their financial activities.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,13 +208,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="7"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
       <sz val="7"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -226,7 +228,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -250,37 +252,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FFACA899"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FFACA899"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFACA899"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FFACA899"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFACA899"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="medium">
         <color rgb="FFACA899"/>
@@ -295,18 +266,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,25 +554,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H2" sqref="A1:H19"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H18" sqref="A1:H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="5"/>
+    <row r="1" spans="1:8" ht="336.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="2" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -616,24 +597,24 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
         <v>3</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1">
-        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>0</v>
@@ -642,16 +623,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
@@ -659,25 +640,25 @@
     </row>
     <row r="4" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
@@ -685,25 +666,25 @@
     </row>
     <row r="5" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="H5" s="1">
         <v>0</v>
@@ -711,25 +692,25 @@
     </row>
     <row r="6" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H6" s="1">
         <v>0</v>
@@ -737,25 +718,25 @@
     </row>
     <row r="7" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H7" s="1">
         <v>0</v>
@@ -763,25 +744,25 @@
     </row>
     <row r="8" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H8" s="1">
         <v>0</v>
@@ -789,51 +770,51 @@
     </row>
     <row r="9" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="307.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>10</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>1</v>
-      </c>
       <c r="D10" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="H10" s="1">
         <v>0</v>
@@ -841,25 +822,25 @@
     </row>
     <row r="11" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H11" s="1">
         <v>0</v>
@@ -867,25 +848,25 @@
     </row>
     <row r="12" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H12" s="1">
         <v>0</v>
@@ -893,25 +874,25 @@
     </row>
     <row r="13" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="H13" s="1">
         <v>0</v>
@@ -919,25 +900,25 @@
     </row>
     <row r="14" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="H14" s="1">
         <v>0</v>
@@ -945,77 +926,77 @@
     </row>
     <row r="15" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="384.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1" t="s">
+      <c r="D16" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="355.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>17</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -1023,53 +1004,39 @@
     </row>
     <row r="18" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="H18" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H19" s="6"/>
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>